<commit_message>
added Adkins design method options, fixed GUI size problem (optimization scroll area), other bugs
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -124,31 +124,172 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Scatter Chart1</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Turbine info'!$A$11:$A$22</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Turbine info'!$B$10:$B$22</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <scatterChart>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Turbine info'!$A$11:$A$22</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Turbine info'!$C$10:$C$22</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Size1</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Percentage1</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+        <crosses val="max"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>4</col>
       <colOff>0</colOff>
-      <row>1</row>
+      <row>0</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="6096000" cy="4572000"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="1" name="Image 1" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
     <clientData/>
   </oneCellAnchor>
 </wsDr>

</xml_diff>